<commit_message>
Riesecuzione di tutti i test per l'accreditamento e aggiornamento dei riferimenti all'interno dei file checklist e data.json.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1111MEDUSASOFTX/Medusa_Software/Urania_FSE/v.2.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1111MEDUSASOFTX/Medusa_Software/Urania_FSE/v.2.0.0/report-checklist.xlsx
@@ -292,13 +292,13 @@
 </t>
   </si>
   <si>
-    <t>2025-04-17T07:47:10Z</t>
-  </si>
-  <si>
-    <t>7ef31d4c27c550a922af82ae2513f3b4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.d9999a1039^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T07:53:49Z</t>
+  </si>
+  <si>
+    <t>ce44f48998f9cc0ba5a7fb19083acae3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.aa2c7c645a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -400,10 +400,10 @@
     </r>
   </si>
   <si>
-    <t>2025-04-17T07:57:23Z</t>
-  </si>
-  <si>
-    <t>396038ee88be0ea80083df240f9f56de</t>
+    <t>2025-05-07T07:59:02Z</t>
+  </si>
+  <si>
+    <t>4cc50eca7d638eb1efacd6bdc16b88a6</t>
   </si>
   <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
@@ -426,10 +426,10 @@
     <t>VALIDAZIONE_TOKEN_JWT_LDO_KO</t>
   </si>
   <si>
-    <t>2025-04-18T14:23:04Z</t>
-  </si>
-  <si>
-    <t>77f541f899cb09a4f7f22aac921c4a9f</t>
+    <t>2025-05-07T08:09:51Z</t>
+  </si>
+  <si>
+    <t>ddfcae7b77c717633b93f5beafca639d</t>
   </si>
   <si>
     <t>RAD</t>
@@ -438,10 +438,10 @@
     <t>VALIDAZIONE_TOKEN_JWT_RAD_KO</t>
   </si>
   <si>
-    <t>2025-04-18T13:05:14Z</t>
-  </si>
-  <si>
-    <t>231fa3f23022153094c38dc185adca3e</t>
+    <t>2025-05-07T08:13:07Z</t>
+  </si>
+  <si>
+    <t>c9ea4d59005e8ef1b6b6d1aa0ee821dc</t>
   </si>
   <si>
     <t>RSA</t>
@@ -450,10 +450,10 @@
     <t>VALIDAZIONE_TOKEN_JWT_RSA_KO</t>
   </si>
   <si>
-    <t>2025-04-18T05:37:44Z</t>
-  </si>
-  <si>
-    <t>e891226904c5dfaaaf287dbdcef128dd</t>
+    <t>2025-05-07T08:15:02Z</t>
+  </si>
+  <si>
+    <t>67bf3e0520772363c66f7ec412830b4f</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_LAB_KO</t>
@@ -543,10 +543,10 @@
     </r>
   </si>
   <si>
-    <t>2025-04-17T08:06:12Z</t>
-  </si>
-  <si>
-    <t>8766b83c213eebfcdd3e0328b30f27f9</t>
+    <t>2025-05-07T08:16:48Z</t>
+  </si>
+  <si>
+    <t>4dad1f95636d5d3331e8f1dc3b736238</t>
   </si>
   <si>
     <t>"type":"/msg/jwt-validation","title":"Campo token JWT non valido.","detail":"Il campo action_id non è corretto","status":403,"instance":"/jwt-mandatory-field-malformed"</t>
@@ -555,28 +555,28 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_LDO_KO</t>
   </si>
   <si>
-    <t>2025-04-18T14:25:32Z</t>
-  </si>
-  <si>
-    <t>2344e9a5de39f2070738f5b81e400860</t>
+    <t>2025-05-07T08:18:34Z</t>
+  </si>
+  <si>
+    <t>630086c0d554fa06057d3b2892536758</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RAD_KO</t>
   </si>
   <si>
-    <t>2025-04-18T13:08:33Z</t>
-  </si>
-  <si>
-    <t>03e8d7974d8677e184ba1cdf773a1e8f</t>
+    <t>2025-05-07T08:19:42Z</t>
+  </si>
+  <si>
+    <t>47210c241055712c06ad6d7a5231b32a</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RSA_KO</t>
   </si>
   <si>
-    <t>2025-04-18T05:52:58Z</t>
-  </si>
-  <si>
-    <t>cc881ab8c0c11dcaee99e1b8010970e5</t>
+    <t>2025-05-07T08:22:24Z</t>
+  </si>
+  <si>
+    <t>3e51a22de8ecf15be881b9e989299af2</t>
   </si>
   <si>
     <t>VALIDAZIONE_LAB_TIMEOUT</t>
@@ -610,13 +610,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-17T08:34:32Z</t>
-  </si>
-  <si>
-    <t>8198fe2a6b10ced5d2c15d161bafd348</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.7b6debe97e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T08:29:21Z</t>
+  </si>
+  <si>
+    <t>91514a1cbe93168d5f8e4e46c2593eea</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.8dc9b920da^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-12| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ],[W002 | Si consiglia di valorizzare l'elemento organizer[CLUSTER]/code]","status":422,"instance":"/validation/error"</t>
@@ -636,13 +636,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-17T08:41:16Z</t>
-  </si>
-  <si>
-    <t>05d348a5ea6812c8e4ab2971ad1a15de</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.be8de01efa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T08:32:57Z</t>
+  </si>
+  <si>
+    <t>1ac5738b926778d4c893051ac732aa1d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.8b8fb7e917^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-15| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family'],[W002 | Si consiglia di valorizzare l'elemento organizer[CLUSTER]/code]","status":422,"instance":"/validation/error"</t>
@@ -655,13 +655,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-17T08:46:40Z</t>
-  </si>
-  <si>
-    <t>4e54a3a25fcd633e938a477d18e74e9d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.7efabdefb6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T08:34:09Z</t>
+  </si>
+  <si>
+    <t>52cb64859c930111ffd3d796380cf11a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.f8aa5f0f9a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/vocabulary","title":"Errore vocabolario.","detail":"Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: NB]","status":400,"instance":"/validation/error"</t>
@@ -681,13 +681,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-17T12:59:36Z</t>
-  </si>
-  <si>
-    <t>5dd37b790ba92183a7dbe3b22c784195</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.f11e6f1ab8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T08:35:20Z</t>
+  </si>
+  <si>
+    <t>9b71557c3caf582dfa383ec241519509</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.ada1fc8c32^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/vocabulary","title":"Errore vocabolario.","detail":"Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.7 v2.1.0, Codes: Z]","status":400,"instance":"/validation/error"</t>
@@ -700,13 +700,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-17T08:53:24Z</t>
-  </si>
-  <si>
-    <t>fca8b9020908f50e971b09ffad7acd26</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.e028d2c04d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T08:36:40Z</t>
+  </si>
+  <si>
+    <t>ed4ab80a38568de655d6da36dace9960</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.8f7c22f7d8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/syntax","title":"Errore di sintassi.","detail":"ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element '{\"urn:hl7-org:v3\":priorityCode}'. One of '{\"urn:hl7-org:v3\":realmCode, \"urn:hl7-org:v3\":typeId, \"urn:hl7-org:v3\":templateId, \"urn:hl7-org:v3\":id}' is expected.","status":400,"instance":"/validation/error"</t>
@@ -719,13 +719,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-17T08:57:15Z</t>
-  </si>
-  <si>
-    <t>6f8d8c2c4a9d4111b56c484bee513941</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.d945b18e6f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T12:25:56Z</t>
+  </si>
+  <si>
+    <t>74a167ce5d82e52e9a113d7c93bcf926</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.191bb41fc1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b1| L'elemento code della section DEVE essere valorizzato con uno dei seguenti codici LOINC individuati:\n\t\t\t\t\t\t18717-9 BANCA DEL SANGUE\n\t\t\t\t\t\t18718-7 MARCATORI CELLULARI \n\t\t\t\t\t\t18719-5 CHIMICA\n\t\t\t\t\t\t18720-3\tCOAGULAZIONE\n\t\t\t\t\t\t18721-1 MONITORAGGIO TERAPEUTICO DEI FARMACI\n\t\t\t\t\t\t18722-9 FERTILITÀ\n\t\t\t\t\t\t18723-7 EMATOLOGIA\n\t\t\t\t\t\t18724-5 HLA\n\t\t\t\t\t\t18725-2 MICROBIOLOGIA\n\t\t\t\t\t\t18727-8 SEROLOGIA\n\t\t\t\t\t\t18728-6 TOSSICOLOGIA\n\t\t\t\t\t\t18729-4 ESAMI DELLE URINE\n\t\t\t\t\t\t18767-4 EMOGASANALISI\n\t\t\t\t\t\t18768-2 CONTE CELLULARE+DIFFERENZIALE\n\t\t\t\t\t\t18769-0 SUSCETTIBILITÀ ANTIMICROBICA\n\t\t\t\t\t\t26435-8 PATOLOGIA MOLECOLARE\n\t\t\t\t\t\t26436-6 ESAMI DI LABORATORIO\n\t\t\t\t\t\t26437-4 TEST DI SENSIBILITÀ A SOSTANZE CHIMICHE\n\t\t\t\t\t\t26438-2 CITOLOGIA\n\t\t\t\t\t\t18716-1 ALLERGOLOGIA\n\t\t\t\t\t\t26439-0 PATOLOGIA CHIRURGICA],[W002 | Si consiglia di valorizzare l'elemento organizer[CLUSTER]/code]","status":422,"instance":"/validation/error"</t>
@@ -738,13 +738,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-17T12:11:40Z</t>
-  </si>
-  <si>
-    <t>e10f4a60497b400f6986711eb48b3019</t>
-  </si>
-  <si>
-    <t>.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.5d782fd004^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T12:27:52Z</t>
+  </si>
+  <si>
+    <t>eff0153243ee49748d7677d0b2beeb1b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.79c5719976^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b10| L'elemento specimen deve contenere l'elemento specimenRole/specimenPlayingEntity ],[ERRORE-b11| L'elemento specimen/specimenRole/specimenPlayingEntity deve contenere l'elemento 'code'],[W002 | Si consiglia di valorizzare l'elemento organizer[CLUSTER]/code]","status":422,"instance":"/validation/error"</t>
@@ -757,13 +757,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-17T12:18:33Z</t>
-  </si>
-  <si>
-    <t>202c42e226d2e3b637ab9466d9542588</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.25c9b8001b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T12:29:33Z</t>
+  </si>
+  <si>
+    <t>c6062efd7fbec9ce414884e8dcc95f24</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.53288e1bc8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b19| L’elemento organizer di tipo 'BATTERY' (@classCode='BATTERY') DEVE contenere l’elemento organizer/code.\n\t\t\t],[W002 | Si consiglia di valorizzare l'elemento organizer[CLUSTER]/code]","status":422,"instance":"/validation/error"</t>
@@ -776,13 +776,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2025-04-18T14:29:08Z</t>
-  </si>
-  <si>
-    <t>5a846c126d6bba05f8f675dc11eac1f0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.c3a5ea5910^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T12:31:01Z</t>
+  </si>
+  <si>
+    <t>a82272dd9d5122fe39deda9fb6b85567</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.31aa007c8c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/jwt-validation","title":"Campo token JWT non valido.","detail":"Il codice fiscale nel campo person_id non è corretto","status":403,"instance":"/jwt-mandatory-field-malformed"</t>
@@ -795,13 +795,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2025-04-18T14:32:13Z</t>
-  </si>
-  <si>
-    <t>c4845b8fef8fe0d185f21f2cdfbf2aa3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.745772ebe4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T12:32:25Z</t>
+  </si>
+  <si>
+    <t>4f222708cb4a4ec4000d793ad9df3840</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.c0011dfb3e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ]","status":422,"instance":"/validation/error"</t>
@@ -814,13 +814,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2025-04-18T14:35:04Z</t>
-  </si>
-  <si>
-    <t>5b28189e07fd1ff9192d80fe2823c1cb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.46aa196192^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T12:33:35Z</t>
+  </si>
+  <si>
+    <t>b89bbd6c4d7c5ebf7f80e3532045499e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.3afdeb9beb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family']","status":422,"instance":"/validation/error"</t>
@@ -833,13 +833,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2025-04-18T14:37:24Z</t>
-  </si>
-  <si>
-    <t>f964c1aba9e4cbc3a7efa401b9f4e674</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.da86ad29b0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T12:34:43Z</t>
+  </si>
+  <si>
+    <t>430506c2b1e298b917b5b15d48a154de</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.8a65cedff1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/vocabulary","title":"Errore vocabolario.","detail":"Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: ND]","status":400,"instance":"/validation/error"</t>
@@ -852,13 +852,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2025-04-18T14:40:00Z</t>
-  </si>
-  <si>
-    <t>55c7f44a7d8361f22646785b3070749b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.009d269f35^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T12:36:13Z</t>
+  </si>
+  <si>
+    <t>568177188a25881c656a275eed17fe80</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.f079d3eb77^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b5| Sezione Condizioni del paziente e diagnosi alla dimissione: la sezione DEVE essere presente],[ERRORE-b6| Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione DEVE contenere l'elemento 'text'],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO' contenere l'elemento 'entry' ]","status":422,"instance":"/validation/error"</t>
@@ -871,13 +871,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2025-04-18T14:42:26Z</t>
-  </si>
-  <si>
-    <t>f9979645f8032805c0e87953bfb464d6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.1c6c7faada^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T12:43:36Z</t>
+  </si>
+  <si>
+    <t>b048ad1c26e097081dd8640be9f4f962</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.0e2b60bdaa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b4| Sezione Decorso Ospedaliero: La sezione deve contenere l'elemento 'text']","status":422,"instance":"/validation/error"</t>
@@ -890,13 +890,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2025-04-18T14:44:44Z</t>
-  </si>
-  <si>
-    <t>d47daf95ffec2c2fa2b4bfdc730dee2a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.9991f4b66b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T12:44:58Z</t>
+  </si>
+  <si>
+    <t>409c35211fce31d601070ad1aadf4588</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.6ffa86aafc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b26| Sotto-sezione Anamnesi: l'elemento entry/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato]","status":422,"instance":"/validation/error"</t>
@@ -909,13 +909,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2025-04-18T14:48:03Z</t>
-  </si>
-  <si>
-    <t>c29a9abc17de46e1cbaeb990f5398d80</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.8d73ffbca6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T12:47:06Z</t>
+  </si>
+  <si>
+    <t>87b24227460ad3090b2c019a8c726749</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.c0dbee0051^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b94|Sezione Terapia farmacologica alla dimissione: section/entry/substanceAdministration/effectiveTime deve avere l'elemento 'low' valorizzato ]","status":422,"instance":"/validation/error"</t>
@@ -928,13 +928,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2025-04-18T14:50:22Z</t>
-  </si>
-  <si>
-    <t>5c9a7a1ff6bb507d206c102deec6557e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.7c9b3de2d6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T12:52:37Z</t>
+  </si>
+  <si>
+    <t>ec025fff22a39ed20efbd50593bb1047</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.4ee419a63d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/vocabulary","title":"Errore vocabolario.","detail":"Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: 999999999]","status":400,"instance":"/validation/error"</t>
@@ -947,13 +947,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2025-04-18T14:53:05Z</t>
-  </si>
-  <si>
-    <t>243714e0acb25eca339e99db0ae6f7df</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.e719a52708^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T12:54:01Z</t>
+  </si>
+  <si>
+    <t>41d7fc5adfbd616be96d03c45dbe2609</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.64f8d553ee^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/vocabulary","title":"Errore vocabolario.","detail":"Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.112 v2.1.0, Codes: 999999999]","status":400,"instance":"/validation/error"</t>
@@ -966,13 +966,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T13:13:21Z</t>
-  </si>
-  <si>
-    <t>4684232774cd7bcf6459641caf2d7f9e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.5b6e35e6ff^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T13:00:45Z</t>
+  </si>
+  <si>
+    <t>18793ec63875eda5daa8a14d76a3584b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.dc59e89c7c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT8_KO</t>
@@ -982,13 +982,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T13:16:47Z</t>
-  </si>
-  <si>
-    <t>350f7c31cbafef7ed436a3213a6cc5fa</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.2c3b9238ba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T13:03:02Z</t>
+  </si>
+  <si>
+    <t>ef19fa01b3495942369d618a1e6bed11</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.c77d6345aa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i suoi sotto-elementi 'country', 'city' e 'streetAddressLine'.   ]","status":422,"instance":"/validation/error"</t>
@@ -1001,13 +1001,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T13:19:55Z</t>
-  </si>
-  <si>
-    <t>6476bb7f56b4118d2a239c3f87336e58</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.1d619c7e9a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T13:04:20Z</t>
+  </si>
+  <si>
+    <t>376074710e71b29a7764e223faad1aea</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.51e39a68eb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i suoi sotto-elementi 'country', 'city' e 'streetAddressLine'.   ],[ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family']","status":422,"instance":"/validation/error"</t>
@@ -1020,13 +1020,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T13:22:51Z</t>
-  </si>
-  <si>
-    <t>1c29ca82ade1bf3a21d723a1a06bd662</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.fa47675ae4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T13:05:58Z</t>
+  </si>
+  <si>
+    <t>7607314e950b802f0df50cbdc076622d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.ab5985def6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT11_KO</t>
@@ -1036,13 +1036,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T13:27:58Z</t>
-  </si>
-  <si>
-    <t>eee7dfd1103188742ed0f0862a1554ce</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.1210a7c2eb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T13:07:24Z</t>
+  </si>
+  <si>
+    <t>da9bd03cc5af517975725536c8ba8cfb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.cd663e4846^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/vocabulary","title":"Errore vocabolario.","detail":"Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.2.9.6.2.7 v1.0.0, Codes: 9999999999]","status":400,"instance":"/validation/error"</t>
@@ -1055,13 +1055,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T13:31:31Z</t>
-  </si>
-  <si>
-    <t>220023f67e9423bd2eae835e220cf6aa</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.a7f1a1a034^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T13:09:20Z</t>
+  </si>
+  <si>
+    <t>66f56045d836defc554e0c089f70aff3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.6a178854e8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT13_KO</t>
@@ -1071,13 +1071,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T13:34:13Z</t>
-  </si>
-  <si>
-    <t>5d0088a005220bd485585227cf062b65</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.b93dc29637^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T13:10:36Z</t>
+  </si>
+  <si>
+    <t>6a9ec59fcf1692b3c2442b0ebcd5420a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.aad6b1d219^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT14_KO</t>
@@ -1087,13 +1087,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T13:37:02Z</t>
-  </si>
-  <si>
-    <t>cc7adca855eb2135bfde47c3583518bf</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.27cec9fea7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T13:11:35Z</t>
+  </si>
+  <si>
+    <t>8a034d0f553ec469f04e94227006c851</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.b733d7b3d0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/syntax","title":"Errore di sintassi.","detail":"ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element '{\"urn:hl7-org:v3\":text}'. One of '{\"urn:hl7-org:v3\":realmCode, \"urn:hl7-org:v3\":typeId, \"urn:hl7-org:v3\":templateId, \"urn:hl7-org:v3\":id, \"urn:hl7-org:v3\":code}' is expected.","status":400,"instance":"/validation/error"</t>
@@ -1106,13 +1106,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T13:39:43Z</t>
-  </si>
-  <si>
-    <t>9526c69481598eef1a5643cb582465be</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.8c9273b82c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T13:13:01Z</t>
+  </si>
+  <si>
+    <t>90d377f7ed78f581ec0f83a1ebe6fb06</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.7eb4199d46^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b4| Sezione Referto: DEVE essere presente la sezione \"Referto\".],[ERRORE-b5| Sezione Referto: La sezione deve contenere l'elemento 'text'.]","status":422,"instance":"/validation/error"</t>
@@ -1125,13 +1125,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T13:42:35Z</t>
-  </si>
-  <si>
-    <t>0abc205342d245757b8ad502c16120d5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.93aa83f4bf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T13:14:11Z</t>
+  </si>
+  <si>
+    <t>644117aca532f6451e49732f95fd4bbf</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.4cb7ebf362^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b13| Sezione Precedenti Esami Eseguiti: La section deve contenere l'elemento 'text'.]","status":422,"instance":"/validation/error"</t>
@@ -1144,13 +1144,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T13:45:11Z</t>
-  </si>
-  <si>
-    <t>b722f3dc12b828103f83cd176ccb0c25</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.5797d5148d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T13:15:24Z</t>
+  </si>
+  <si>
+    <t>96d86481b9cda33be7f5c3dfee9ff012</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.64b5670bc3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b7| Sezione Dicom Object Catalog: La sezione deve avere l'elemento 'entry' di tipo 'act'.]","status":422,"instance":"/validation/error"</t>
@@ -1163,13 +1163,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T13:47:48Z</t>
-  </si>
-  <si>
-    <t>385e064918d907b913f87c94ae37c803</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.ccd6fa21a8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T13:17:20Z</t>
+  </si>
+  <si>
+    <t>9688af4d8cd28134331650c9a77fddd7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.fbb55b9aa3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b22| Sezione Storia Clinica: L'elemento entry/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato.]","status":422,"instance":"/validation/error"</t>
@@ -1182,13 +1182,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T13:50:15Z</t>
-  </si>
-  <si>
-    <t>569bc64e25a8eac2ee4d38a4719cd173</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.8a44b72ade^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T13:20:09Z</t>
+  </si>
+  <si>
+    <t>eb055ec34ee8fc6861c3a65b75e0b336</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.42699f4ce1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b26| Sezione Storia Clinica: La entry/organizer deve avere un elemento subject/relatedSubject il quale deve contenere l'elemento 'code'. ]","status":422,"instance":"/validation/error"</t>
@@ -1201,13 +1201,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T13:53:02Z</t>
-  </si>
-  <si>
-    <t>ce59aa45031803a3052f0ee31c14973d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.afbb0918ed^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T13:21:25Z</t>
+  </si>
+  <si>
+    <t>667c3016af88deb513f53462350c5fd5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.bf3d1e9d7c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b53| Sotto sezione Allergie: I'elemento entry/act/entryRelationship/observation/effectiveTime deve avere valorizzato l'elemento 'low'.]","status":422,"instance":"/validation/error"</t>
@@ -1220,13 +1220,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T13:55:27Z</t>
-  </si>
-  <si>
-    <t>eaa67ca55a6d7465dd90ce04ba9e8223</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.be150052f4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T13:22:22Z</t>
+  </si>
+  <si>
+    <t>12476e374b76ff00d43e8d6d9a285e38</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.6126e23611^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b57| Sotto sezione Allergie: L'elemento entryRelationship/observation (Descrizione Agente) deve avere almeno un elemento 'participant' che dettaglia l'agente scatenante.]","status":422,"instance":"/validation/error"</t>
@@ -1239,13 +1239,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T14:01:03Z</t>
-  </si>
-  <si>
-    <t>29acd38429bbadbfc14bc77c518f1fe4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.c9cfb3847f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T13:23:26Z</t>
+  </si>
+  <si>
+    <t>1d7e196f082b7bc5b91548121ed5b96a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.039d7d5aa1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT23_KO</t>
@@ -1255,13 +1255,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T14:04:06Z</t>
-  </si>
-  <si>
-    <t>bdd3063c87849f906d2567277738375c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.314a7ed388^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T13:24:54Z</t>
+  </si>
+  <si>
+    <t>646ac2e5f00e857b553bd229c5a14eb9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.079f0f4c5b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-40| L'elemento ClinicalDocument/documentationOf/serviceEvent deve contenere l'elemento code e DEVE valorizzare il suo attributo code con uno dei seguenti valori: 'PROG'|'DIR'|'RAD_PROG|'RAD_DIR' ]","status":422,"instance":"/validation/error"</t>
@@ -1274,13 +1274,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T06:00:59Z</t>
-  </si>
-  <si>
-    <t>7e705822aa61527d5588b6c23e597b80</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.2a96168cb7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:03:26Z</t>
+  </si>
+  <si>
+    <t>759ce535b53be559f4c52e409c15ca20</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.af86b7773b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT8_KO</t>
@@ -1290,13 +1290,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T06:05:29Z</t>
-  </si>
-  <si>
-    <t>8f6e2abea53cda8988f4cc3facd79aff</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.9ad6a37de6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:04:59Z</t>
+  </si>
+  <si>
+    <t>434a77e0853974438b76b4a79d5174a0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.520fcd4398^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ]","status":422,"instance":"/validation/error</t>
@@ -1309,13 +1309,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T06:08:57Z</t>
-  </si>
-  <si>
-    <t>dd38953049445da1c4cf965ceaee3324</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.e3f45c349f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:06:01Z</t>
+  </si>
+  <si>
+    <t>a76d5432694f0b5de987859a0cb3cbd1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.fba552b978^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT10_KO</t>
@@ -1325,13 +1325,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T06:11:48Z</t>
-  </si>
-  <si>
-    <t>79f9928d9c0fba65e1e70b66a8c807a0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.f60cc3668a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:07:17Z</t>
+  </si>
+  <si>
+    <t>83d434351a095b0d55ea7960132f590c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.1ba0d7619a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT12_KO</t>
@@ -1341,13 +1341,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T06:16:32Z</t>
-  </si>
-  <si>
-    <t>82302387076b46b2a87f755a2a24f431</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.07f2d414fc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:08:47Z</t>
+  </si>
+  <si>
+    <t>7394039019e2d8c2184ac1ef3a46eb03</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.44d0e64f20^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/vocabulary","title":"Errore vocabolario.","detail":"Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.7 v2.1.0, Codes: DUMMY]","status":400,"instance":"/validation/error"</t>
@@ -1360,13 +1360,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T06:19:32Z</t>
-  </si>
-  <si>
-    <t>4e45d821b319f527fdde83c70ffbc2de</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.36cd6e62ec^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:09:49Z</t>
+  </si>
+  <si>
+    <t>635620fca4731ba87a8b36ac73b4524d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.6d1a440670^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT14_KO</t>
@@ -1376,13 +1376,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T06:22:34Z</t>
-  </si>
-  <si>
-    <t>da097d5761f9901a648aaee510ee2812</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.9edf7903b4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:11:07Z</t>
+  </si>
+  <si>
+    <t>49ccf440473231698b0a33c6ca5f4cec</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.ca251800d2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/syntax","title":"Errore di sintassi.","detail":"ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element '{\"urn:hl7-org:v3\":statusCode}'. One of '{\"urn:hl7-org:v3\":realmCode, \"urn:hl7-org:v3\":typeId, \"urn:hl7-org:v3\":templateId, \"urn:hl7-org:v3\":id, \"urn:hl7-org:v3\":code}' is expected.,ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element '{\"urn:hl7-org:v3\":effectiveTime}'. One of '{\"urn:hl7-org:v3\":realmCode, \"urn:hl7-org:v3\":typeId, \"urn:hl7-org:v3\":templateId, \"urn:hl7-org:v3\":id, \"urn:hl7-org:v3\":code}' is expected.","status":400,"instance":"/validation/error"</t>
@@ -1395,13 +1395,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T06:25:34Z</t>
-  </si>
-  <si>
-    <t>806d4a7123dd6d4e4e63e1943b0ebf9f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.eea4724c1d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:12:14Z</t>
+  </si>
+  <si>
+    <t>bd74d6f343b7ba1864945ad96bbac7ba</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.84dbced293^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b4| Sezione Referto: la sezione DEVE essere presente],[ERRORE-b5| Sezione Referto: la sezione DEVE contenere un elemento 'text']","status":422,"instance":"/validation/error"</t>
@@ -1414,13 +1414,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T06:28:49Z</t>
-  </si>
-  <si>
-    <t>eae9747389096da08059089ba129208d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.f5fca23441^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:14:29Z</t>
+  </si>
+  <si>
+    <t>6d153b848bd5a6545d244d4d1cae8998</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.696a3ddae7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b6| Sezione Quesito Diagnostico: la sezione DEVE contenere un elemento 'text']","status":422,"instance":"/validation/error"</t>
@@ -1433,13 +1433,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T12:24:47Z</t>
-  </si>
-  <si>
-    <t>b6639267d2815c11b26fd876274580fe</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.121eaf8bf5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:15:33Z</t>
+  </si>
+  <si>
+    <t>02264a8d1fc725117beeba75ad38fbe3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.54c0baa2fc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b3| Sezione Prestazioni: la sezione DEVE contenere un elemento 'entry']","status":422,"instance":"/validation/error"</t>
@@ -1452,13 +1452,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T12:27:58Z</t>
-  </si>
-  <si>
-    <t>20173d1fffc47545fb8ef1d49ad9636d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.37b1fab45b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:16:43Z</t>
+  </si>
+  <si>
+    <t>46410381693decd559f00d2b4623d528</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.9fbf0405fb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b26| Sezione Storia Clinica: l'elemento entry/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato],[ERRORE-b27| Sezione Storia Clinica: l'elemento entry/observation/effectiveTime deve essere presente e deve avere l'elemento 'high' valorizzato nel caso in cui il problema risulta non essere più presente]","status":422,"instance":"/validation/error"</t>
@@ -1471,13 +1471,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T12:33:22Z</t>
-  </si>
-  <si>
-    <t>550f562421831bd080eae81fa28135c6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.e9b18ea137^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:17:56Z</t>
+  </si>
+  <si>
+    <t>7785da3f2e9935e0e21f1f8f3a4ef64e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.c0520e9e9e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b36| Sezione Storia Clinica: l'elemento entry/organizer/subject/relatedSubject deve avere l'attributo @classCode='PRS' e deve contenere l'elemento 'code']","status":422,"instance":"/validation/error"</t>
@@ -1490,13 +1490,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T12:36:56Z</t>
-  </si>
-  <si>
-    <t>e159418a2a21cb84676e310b6ecc1400</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.6c6bc251e3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:19:01Z</t>
+  </si>
+  <si>
+    <t>ac903e18d345aa9016c2800a0126c6ba</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.2a5c6a521d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b53| Sotto-sezione Allergie: l'elemento entry/act/entryRelationship/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato ]","status":422,"instance":"/validation/error"</t>
@@ -1509,13 +1509,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T12:39:17Z</t>
-  </si>
-  <si>
-    <t>a3fbe77372108f5c2b0b0aa386424658</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.07082ef9a2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:20:06Z</t>
+  </si>
+  <si>
+    <t>8ccac8dc8c1f1409ddc8312a010a52ad</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.df9af36a4c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-b57| Sotto-sezione Allergie: entry/act/entryRelationship/observation deve contenere almeno un elemento 'participant']","status":422,"instance":"/validation/error"</t>
@@ -1528,13 +1528,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T12:41:39Z</t>
-  </si>
-  <si>
-    <t>23964ab26332388b02e8dcb4ca34cb66</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.41b82c9f1b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:21:24Z</t>
+  </si>
+  <si>
+    <t>2f5e42e7954440eac017482b48b4e4e1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.26d11780c8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/vocabulary","title":"Errore vocabolario.","detail":"Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: 69.69.69]","status":400,"instance":"/validation/error"</t>
@@ -1547,13 +1547,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T12:44:46Z</t>
-  </si>
-  <si>
-    <t>38a062e4ef9698fba866573aa1abf85b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.25736d2f75^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:22:30Z</t>
+  </si>
+  <si>
+    <t>dd8ea24ae36277135e7d78a0a004f151</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.66590f8c57^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/semantic","title":"Errore semantico.","detail":"[ERRORE-30| L'elemento ClinicalDocument/legalAuthenticator/signatureCode deve essere valorizzato con il codice \"S\" ]","status":422,"instance":"/validation/error"</t>
@@ -1588,13 +1588,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T12:57:18Z</t>
-  </si>
-  <si>
-    <t>fd9cb4028b5d0c5bfd8a2d048e140ec9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.a0459fbfd7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:24:54Z</t>
+  </si>
+  <si>
+    <t>c9775173d5f71e061980cf690272ec47</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.f97d023067^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT2</t>
@@ -1604,13 +1604,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T13:01:25Z</t>
-  </si>
-  <si>
-    <t>1a97a311208b3e6db8ea24aa89fe5e96</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.fa6b12fe7f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:26:12Z</t>
+  </si>
+  <si>
+    <t>a3281d09f42a4e9d4c1a52ee53b34b78</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.d91031032a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT24</t>
@@ -1620,13 +1620,13 @@
 Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 24" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T05:40:10Z</t>
-  </si>
-  <si>
-    <t>963c7719f1e433e721b9f691531cf743</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.475ce39849^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:27:37Z</t>
+  </si>
+  <si>
+    <t>6c28a99aa69a985611b5f2f9a5e65e92</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.c5dd905cd7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT25</t>
@@ -1636,13 +1636,13 @@
 Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 25" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T05:49:45Z</t>
-  </si>
-  <si>
-    <t>91fe757cd31a1cf77ab96f754a394238</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.d948e5b257^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:29:01Z</t>
+  </si>
+  <si>
+    <t>3789a798225be7b1717480dcf59d0f2c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.73ec0f2df2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT17</t>
@@ -1652,13 +1652,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 17" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T14:15:50Z</t>
-  </si>
-  <si>
-    <t>770c641ae7fd7050195340985d8823f2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.0103faa5f6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:30:53Z</t>
+  </si>
+  <si>
+    <t>a9b5c09269099d7bdbac5f95498dcd9c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.e019f83c76^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT18</t>
@@ -1668,13 +1668,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 18" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T14:18:39Z</t>
-  </si>
-  <si>
-    <t>6f0c7fbfcc08a37e2a8d5b49517223e9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.889cded565^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:32:24Z</t>
+  </si>
+  <si>
+    <t>70f44d0512f4bec1bd0306817ae7e6b1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.970972a992^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT17</t>
@@ -1685,13 +1685,13 @@
 </t>
   </si>
   <si>
-    <t>2025-04-17T12:28:23Z</t>
-  </si>
-  <si>
-    <t>fb52eecf311ce392</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.97bb3fc5bee3032679f4f07419e04af6375baafa17024527a98ede920c6812ed.27d5ff79ca^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:34:26Z</t>
+  </si>
+  <si>
+    <t>038c99bdbe4d278adf1b993e150bb79f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.97bb3fc5bee3032679f4f07419e04af6375baafa17024527a98ede920c6812ed.31b2baeed8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT26_KO</t>
@@ -1701,13 +1701,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 26" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T12:48:44Z</t>
-  </si>
-  <si>
-    <t>2348ce906cf403e5aa8e31998143912c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.edcad70538^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:35:45Z</t>
+  </si>
+  <si>
+    <t>5bee66151bd7d7010c036153813d72fd</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.20aa8df361^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT24_KO</t>
@@ -1717,13 +1717,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 24" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T14:07:59Z</t>
-  </si>
-  <si>
-    <t>2c92fc3da1459bc6ced8e8b912d31957</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.e2a718b0f3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:37:01Z</t>
+  </si>
+  <si>
+    <t>ea5a2550239d692513bfd01767b15d99</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.fcd383e04d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"type":"/msg/syntax","title":"Errore di sintassi.","detail":"ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element '{\"urn:hl7-org:v3\":languageCode}'. One of '{\"urn:hl7-org:v3\":confidentialityCode}' is expected.","status":400,"instance":"/validation/error"</t>
@@ -1736,13 +1736,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test SING_VACC" e "CDA2_Scheda_Singola Vaccinazione_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-17T12:49:12Z</t>
-  </si>
-  <si>
-    <t>ae85292b947beee4c0f53dff66a21f7b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.77d57c3d03^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:38:11Z</t>
+  </si>
+  <si>
+    <t>e16df92c5fa9c058f2293d5a333fe7e6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.306843f138^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT19_KO</t>
@@ -1752,13 +1752,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2025-04-18T14:56:11Z</t>
-  </si>
-  <si>
-    <t>3fcb215e117ceace27a8e16fcdb9ac0d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.825d104a82^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:39:34Z</t>
+  </si>
+  <si>
+    <t>b69617dc7a10b807f64f3e115a87b89d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.46bed4320e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT27_KO</t>
@@ -1768,13 +1768,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 27" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-04-18T12:53:31Z</t>
-  </si>
-  <si>
-    <t>fe38481b482ef2455b74533badb088ca</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.ffbd023f3a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-07T19:40:44Z</t>
+  </si>
+  <si>
+    <t>be69131a703682ec708d9680cb5dcf8d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.1761460a7e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>LISTA VALORI</t>
@@ -2619,7 +2619,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -2808,9 +2808,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -4352,18 +4349,26 @@
   <cols>
     <col min="1" max="1" width="7.65625" style="25" customWidth="1"/>
     <col min="2" max="2" width="15.5781" style="25" customWidth="1"/>
-    <col min="3" max="3" width="14.9297" style="25" customWidth="1"/>
-    <col min="4" max="4" width="46.125" style="25" customWidth="1"/>
-    <col min="5" max="5" width="104.852" style="25" customWidth="1"/>
-    <col min="6" max="9" width="33.1719" style="25" customWidth="1"/>
-    <col min="10" max="10" width="27.1719" style="25" customWidth="1"/>
-    <col min="11" max="11" width="30" style="25" customWidth="1"/>
-    <col min="12" max="12" width="31.6719" style="25" customWidth="1"/>
-    <col min="13" max="18" width="36.5" style="25" customWidth="1"/>
+    <col min="3" max="3" width="6.86719" style="25" customWidth="1"/>
+    <col min="4" max="4" width="33.1484" style="25" customWidth="1"/>
+    <col min="5" max="5" width="95.8672" style="25" customWidth="1"/>
+    <col min="6" max="6" width="12.7344" style="25" customWidth="1"/>
+    <col min="7" max="7" width="20.5469" style="25" customWidth="1"/>
+    <col min="8" max="9" width="33.1719" style="25" customWidth="1"/>
+    <col min="10" max="10" width="12.4375" style="25" customWidth="1"/>
+    <col min="11" max="11" width="16" style="25" customWidth="1"/>
+    <col min="12" max="12" width="17.9141" style="25" customWidth="1"/>
+    <col min="13" max="13" width="18.3672" style="25" customWidth="1"/>
+    <col min="14" max="14" width="16.3125" style="25" customWidth="1"/>
+    <col min="15" max="15" width="36.5" style="25" customWidth="1"/>
+    <col min="16" max="16" width="15.7656" style="25" customWidth="1"/>
+    <col min="17" max="17" width="14.5469" style="25" customWidth="1"/>
+    <col min="18" max="18" width="14.9297" style="25" customWidth="1"/>
     <col min="19" max="19" width="27.1719" style="25" customWidth="1"/>
-    <col min="20" max="20" width="33.1719" style="25" customWidth="1"/>
-    <col min="21" max="21" width="36.5" style="25" customWidth="1"/>
-    <col min="22" max="23" width="31.8516" style="25" customWidth="1"/>
+    <col min="20" max="20" width="14.2812" style="25" customWidth="1"/>
+    <col min="21" max="21" width="15.1016" style="25" customWidth="1"/>
+    <col min="22" max="22" width="14.8984" style="25" customWidth="1"/>
+    <col min="23" max="23" width="31.8516" style="25" customWidth="1"/>
     <col min="24" max="16384" width="14.5" style="25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4667,7 +4672,7 @@
         <v>58</v>
       </c>
       <c r="F10" s="57">
-        <v>45764</v>
+        <v>45784</v>
       </c>
       <c r="G10" t="s" s="58">
         <v>59</v>
@@ -4726,7 +4731,7 @@
         <v>67</v>
       </c>
       <c r="F11" s="57">
-        <v>45764</v>
+        <v>45784</v>
       </c>
       <c r="G11" t="s" s="58">
         <v>68</v>
@@ -4789,7 +4794,7 @@
         <v>67</v>
       </c>
       <c r="F12" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G12" t="s" s="58">
         <v>76</v>
@@ -4852,7 +4857,7 @@
         <v>67</v>
       </c>
       <c r="F13" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G13" t="s" s="58">
         <v>80</v>
@@ -4915,7 +4920,7 @@
         <v>67</v>
       </c>
       <c r="F14" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G14" t="s" s="58">
         <v>84</v>
@@ -4978,7 +4983,7 @@
         <v>87</v>
       </c>
       <c r="F15" s="57">
-        <v>45764</v>
+        <v>45784</v>
       </c>
       <c r="G15" t="s" s="58">
         <v>88</v>
@@ -5041,7 +5046,7 @@
         <v>87</v>
       </c>
       <c r="F16" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G16" t="s" s="58">
         <v>92</v>
@@ -5104,7 +5109,7 @@
         <v>87</v>
       </c>
       <c r="F17" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G17" t="s" s="58">
         <v>95</v>
@@ -5167,7 +5172,7 @@
         <v>87</v>
       </c>
       <c r="F18" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G18" t="s" s="58">
         <v>98</v>
@@ -5230,10 +5235,10 @@
         <v>101</v>
       </c>
       <c r="F19" s="57">
-        <v>45764</v>
+        <v>45784</v>
       </c>
       <c r="G19" t="s" s="58">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="H19" s="57"/>
       <c r="I19" s="57"/>
@@ -5291,10 +5296,10 @@
         <v>101</v>
       </c>
       <c r="F20" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G20" t="s" s="58">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="H20" s="57"/>
       <c r="I20" s="57"/>
@@ -5352,7 +5357,7 @@
         <v>101</v>
       </c>
       <c r="F21" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G21" t="s" s="58">
         <v>98</v>
@@ -5413,7 +5418,7 @@
         <v>101</v>
       </c>
       <c r="F22" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G22" t="s" s="58">
         <v>98</v>
@@ -5474,7 +5479,7 @@
         <v>108</v>
       </c>
       <c r="F23" s="57">
-        <v>45764</v>
+        <v>45784</v>
       </c>
       <c r="G23" t="s" s="58">
         <v>109</v>
@@ -5537,7 +5542,7 @@
         <v>115</v>
       </c>
       <c r="F24" s="57">
-        <v>45764</v>
+        <v>45784</v>
       </c>
       <c r="G24" t="s" s="58">
         <v>116</v>
@@ -5600,7 +5605,7 @@
         <v>121</v>
       </c>
       <c r="F25" s="57">
-        <v>45764</v>
+        <v>45784</v>
       </c>
       <c r="G25" t="s" s="58">
         <v>122</v>
@@ -5663,7 +5668,7 @@
         <v>128</v>
       </c>
       <c r="F26" s="57">
-        <v>45764</v>
+        <v>45784</v>
       </c>
       <c r="G26" t="s" s="58">
         <v>129</v>
@@ -5724,7 +5729,7 @@
         <v>134</v>
       </c>
       <c r="F27" s="57">
-        <v>45764</v>
+        <v>45784</v>
       </c>
       <c r="G27" t="s" s="58">
         <v>135</v>
@@ -5787,7 +5792,7 @@
         <v>140</v>
       </c>
       <c r="F28" s="57">
-        <v>45764</v>
+        <v>45784</v>
       </c>
       <c r="G28" t="s" s="58">
         <v>141</v>
@@ -5850,7 +5855,7 @@
         <v>146</v>
       </c>
       <c r="F29" s="57">
-        <v>45764</v>
+        <v>45784</v>
       </c>
       <c r="G29" t="s" s="58">
         <v>147</v>
@@ -5913,7 +5918,7 @@
         <v>152</v>
       </c>
       <c r="F30" s="57">
-        <v>45764</v>
+        <v>45784</v>
       </c>
       <c r="G30" t="s" s="58">
         <v>153</v>
@@ -5976,7 +5981,7 @@
         <v>158</v>
       </c>
       <c r="F31" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G31" t="s" s="58">
         <v>159</v>
@@ -6039,7 +6044,7 @@
         <v>164</v>
       </c>
       <c r="F32" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G32" t="s" s="58">
         <v>165</v>
@@ -6102,7 +6107,7 @@
         <v>170</v>
       </c>
       <c r="F33" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G33" t="s" s="58">
         <v>171</v>
@@ -6165,7 +6170,7 @@
         <v>176</v>
       </c>
       <c r="F34" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G34" t="s" s="58">
         <v>177</v>
@@ -6228,7 +6233,7 @@
         <v>182</v>
       </c>
       <c r="F35" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G35" t="s" s="58">
         <v>183</v>
@@ -6291,7 +6296,7 @@
         <v>188</v>
       </c>
       <c r="F36" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G36" t="s" s="58">
         <v>189</v>
@@ -6354,7 +6359,7 @@
         <v>194</v>
       </c>
       <c r="F37" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G37" t="s" s="58">
         <v>195</v>
@@ -6417,7 +6422,7 @@
         <v>200</v>
       </c>
       <c r="F38" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G38" t="s" s="58">
         <v>201</v>
@@ -6480,7 +6485,7 @@
         <v>206</v>
       </c>
       <c r="F39" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G39" t="s" s="58">
         <v>207</v>
@@ -6543,7 +6548,7 @@
         <v>212</v>
       </c>
       <c r="F40" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G40" t="s" s="58">
         <v>213</v>
@@ -6606,7 +6611,7 @@
         <v>218</v>
       </c>
       <c r="F41" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G41" t="s" s="58">
         <v>219</v>
@@ -6669,7 +6674,7 @@
         <v>223</v>
       </c>
       <c r="F42" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G42" t="s" s="58">
         <v>224</v>
@@ -6732,7 +6737,7 @@
         <v>229</v>
       </c>
       <c r="F43" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G43" t="s" s="58">
         <v>230</v>
@@ -6795,7 +6800,7 @@
         <v>235</v>
       </c>
       <c r="F44" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G44" t="s" s="58">
         <v>236</v>
@@ -6858,7 +6863,7 @@
         <v>240</v>
       </c>
       <c r="F45" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G45" t="s" s="58">
         <v>241</v>
@@ -6921,7 +6926,7 @@
         <v>246</v>
       </c>
       <c r="F46" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G46" t="s" s="58">
         <v>247</v>
@@ -6984,7 +6989,7 @@
         <v>251</v>
       </c>
       <c r="F47" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G47" t="s" s="58">
         <v>252</v>
@@ -7047,7 +7052,7 @@
         <v>256</v>
       </c>
       <c r="F48" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G48" t="s" s="58">
         <v>257</v>
@@ -7110,7 +7115,7 @@
         <v>262</v>
       </c>
       <c r="F49" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G49" t="s" s="58">
         <v>263</v>
@@ -7173,7 +7178,7 @@
         <v>268</v>
       </c>
       <c r="F50" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G50" t="s" s="58">
         <v>269</v>
@@ -7236,7 +7241,7 @@
         <v>274</v>
       </c>
       <c r="F51" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G51" t="s" s="58">
         <v>275</v>
@@ -7299,7 +7304,7 @@
         <v>280</v>
       </c>
       <c r="F52" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G52" t="s" s="58">
         <v>281</v>
@@ -7362,7 +7367,7 @@
         <v>286</v>
       </c>
       <c r="F53" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G53" t="s" s="58">
         <v>287</v>
@@ -7425,7 +7430,7 @@
         <v>292</v>
       </c>
       <c r="F54" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G54" t="s" s="58">
         <v>293</v>
@@ -7488,7 +7493,7 @@
         <v>298</v>
       </c>
       <c r="F55" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G55" t="s" s="58">
         <v>299</v>
@@ -7551,7 +7556,7 @@
         <v>304</v>
       </c>
       <c r="F56" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G56" t="s" s="58">
         <v>305</v>
@@ -7614,7 +7619,7 @@
         <v>309</v>
       </c>
       <c r="F57" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G57" t="s" s="58">
         <v>310</v>
@@ -7677,7 +7682,7 @@
         <v>315</v>
       </c>
       <c r="F58" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G58" t="s" s="58">
         <v>316</v>
@@ -7740,7 +7745,7 @@
         <v>320</v>
       </c>
       <c r="F59" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G59" t="s" s="58">
         <v>321</v>
@@ -7803,7 +7808,7 @@
         <v>326</v>
       </c>
       <c r="F60" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G60" t="s" s="58">
         <v>327</v>
@@ -7866,7 +7871,7 @@
         <v>331</v>
       </c>
       <c r="F61" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G61" t="s" s="58">
         <v>332</v>
@@ -7929,7 +7934,7 @@
         <v>336</v>
       </c>
       <c r="F62" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G62" t="s" s="58">
         <v>337</v>
@@ -7992,7 +7997,7 @@
         <v>342</v>
       </c>
       <c r="F63" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G63" t="s" s="58">
         <v>343</v>
@@ -8055,7 +8060,7 @@
         <v>347</v>
       </c>
       <c r="F64" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G64" t="s" s="58">
         <v>348</v>
@@ -8118,7 +8123,7 @@
         <v>353</v>
       </c>
       <c r="F65" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G65" t="s" s="58">
         <v>354</v>
@@ -8181,7 +8186,7 @@
         <v>359</v>
       </c>
       <c r="F66" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G66" t="s" s="58">
         <v>360</v>
@@ -8244,7 +8249,7 @@
         <v>365</v>
       </c>
       <c r="F67" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G67" t="s" s="58">
         <v>366</v>
@@ -8307,7 +8312,7 @@
         <v>371</v>
       </c>
       <c r="F68" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G68" t="s" s="58">
         <v>372</v>
@@ -8370,7 +8375,7 @@
         <v>377</v>
       </c>
       <c r="F69" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G69" t="s" s="58">
         <v>378</v>
@@ -8433,7 +8438,7 @@
         <v>383</v>
       </c>
       <c r="F70" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G70" t="s" s="58">
         <v>384</v>
@@ -8496,7 +8501,7 @@
         <v>389</v>
       </c>
       <c r="F71" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G71" t="s" s="58">
         <v>390</v>
@@ -8559,7 +8564,7 @@
         <v>395</v>
       </c>
       <c r="F72" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G72" t="s" s="58">
         <v>396</v>
@@ -8622,7 +8627,7 @@
         <v>401</v>
       </c>
       <c r="F73" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G73" t="s" s="58">
         <v>402</v>
@@ -8771,7 +8776,7 @@
         <v>413</v>
       </c>
       <c r="F76" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G76" t="s" s="58">
         <v>414</v>
@@ -8830,7 +8835,7 @@
         <v>418</v>
       </c>
       <c r="F77" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G77" t="s" s="58">
         <v>419</v>
@@ -8889,7 +8894,7 @@
         <v>423</v>
       </c>
       <c r="F78" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G78" t="s" s="58">
         <v>424</v>
@@ -8948,7 +8953,7 @@
         <v>428</v>
       </c>
       <c r="F79" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G79" t="s" s="58">
         <v>429</v>
@@ -9007,7 +9012,7 @@
         <v>433</v>
       </c>
       <c r="F80" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G80" t="s" s="58">
         <v>434</v>
@@ -9066,7 +9071,7 @@
         <v>438</v>
       </c>
       <c r="F81" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G81" t="s" s="58">
         <v>439</v>
@@ -9125,7 +9130,7 @@
         <v>443</v>
       </c>
       <c r="F82" s="57">
-        <v>45764</v>
+        <v>45784</v>
       </c>
       <c r="G82" t="s" s="58">
         <v>444</v>
@@ -9184,7 +9189,7 @@
         <v>448</v>
       </c>
       <c r="F83" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G83" t="s" s="58">
         <v>449</v>
@@ -9247,7 +9252,7 @@
         <v>453</v>
       </c>
       <c r="F84" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G84" t="s" s="58">
         <v>454</v>
@@ -9310,9 +9315,9 @@
         <v>459</v>
       </c>
       <c r="F85" s="57">
-        <v>45764</v>
-      </c>
-      <c r="G85" t="s" s="63">
+        <v>45784</v>
+      </c>
+      <c r="G85" t="s" s="58">
         <v>460</v>
       </c>
       <c r="H85" t="s" s="55">
@@ -9373,7 +9378,7 @@
         <v>464</v>
       </c>
       <c r="F86" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G86" t="s" s="58">
         <v>465</v>
@@ -9436,7 +9441,7 @@
         <v>469</v>
       </c>
       <c r="F87" s="57">
-        <v>45765</v>
+        <v>45784</v>
       </c>
       <c r="G87" t="s" s="58">
         <v>470</v>
@@ -9488,24 +9493,24 @@
       <c r="C88" s="24"/>
       <c r="D88" s="24"/>
       <c r="E88" s="24"/>
-      <c r="F88" s="64"/>
-      <c r="G88" s="64"/>
-      <c r="H88" s="64"/>
-      <c r="I88" s="64"/>
-      <c r="J88" s="65"/>
-      <c r="K88" s="65"/>
-      <c r="L88" s="65"/>
-      <c r="M88" s="65"/>
-      <c r="N88" s="65"/>
-      <c r="O88" s="65"/>
-      <c r="P88" s="65"/>
-      <c r="Q88" s="65"/>
-      <c r="R88" s="65"/>
-      <c r="S88" s="65"/>
-      <c r="T88" s="65"/>
-      <c r="U88" s="66"/>
-      <c r="V88" s="67"/>
-      <c r="W88" s="68"/>
+      <c r="F88" s="63"/>
+      <c r="G88" s="63"/>
+      <c r="H88" s="63"/>
+      <c r="I88" s="63"/>
+      <c r="J88" s="64"/>
+      <c r="K88" s="64"/>
+      <c r="L88" s="64"/>
+      <c r="M88" s="64"/>
+      <c r="N88" s="64"/>
+      <c r="O88" s="64"/>
+      <c r="P88" s="64"/>
+      <c r="Q88" s="64"/>
+      <c r="R88" s="64"/>
+      <c r="S88" s="64"/>
+      <c r="T88" s="64"/>
+      <c r="U88" s="65"/>
+      <c r="V88" s="66"/>
+      <c r="W88" s="67"/>
     </row>
     <row r="89" ht="14.25" customHeight="1">
       <c r="A89" s="8"/>
@@ -23521,12 +23526,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="8.85156" style="69" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="69" customWidth="1"/>
+    <col min="1" max="5" width="8.85156" style="68" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="68" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="70">
+      <c r="A1" t="s" s="69">
         <v>474</v>
       </c>
       <c r="B1" s="8"/>
@@ -23535,7 +23540,7 @@
       <c r="E1" s="8"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="70">
+      <c r="A2" t="s" s="69">
         <v>475</v>
       </c>
       <c r="B2" s="8"/>
@@ -23544,7 +23549,7 @@
       <c r="E2" s="8"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="70">
+      <c r="A3" t="s" s="69">
         <v>476</v>
       </c>
       <c r="B3" s="8"/>
@@ -23553,7 +23558,7 @@
       <c r="E3" s="8"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="70">
+      <c r="A4" t="s" s="69">
         <v>477</v>
       </c>
       <c r="B4" s="8"/>
@@ -23562,7 +23567,7 @@
       <c r="E4" s="8"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="70">
+      <c r="A5" t="s" s="69">
         <v>478</v>
       </c>
       <c r="B5" s="8"/>
@@ -23571,7 +23576,7 @@
       <c r="E5" s="8"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="70">
+      <c r="A6" t="s" s="69">
         <v>479</v>
       </c>
       <c r="B6" s="8"/>
@@ -23580,7 +23585,7 @@
       <c r="E6" s="8"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="70">
+      <c r="A7" t="s" s="69">
         <v>480</v>
       </c>
       <c r="B7" s="8"/>
@@ -23589,7 +23594,7 @@
       <c r="E7" s="8"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" t="s" s="70">
+      <c r="A8" t="s" s="69">
         <v>408</v>
       </c>
       <c r="B8" s="8"/>
@@ -23628,48 +23633,48 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="71" customWidth="1"/>
-    <col min="2" max="2" width="23.8516" style="71" customWidth="1"/>
-    <col min="3" max="3" width="33.8516" style="71" customWidth="1"/>
-    <col min="4" max="4" width="102" style="71" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="71" customWidth="1"/>
-    <col min="6" max="6" width="9.5" style="71" customWidth="1"/>
-    <col min="7" max="7" width="7.85156" style="71" customWidth="1"/>
-    <col min="8" max="16384" width="14.5" style="71" customWidth="1"/>
+    <col min="1" max="1" width="16" style="70" customWidth="1"/>
+    <col min="2" max="2" width="23.8516" style="70" customWidth="1"/>
+    <col min="3" max="3" width="33.8516" style="70" customWidth="1"/>
+    <col min="4" max="4" width="102" style="70" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="70" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="70" customWidth="1"/>
+    <col min="7" max="7" width="7.85156" style="70" customWidth="1"/>
+    <col min="8" max="16384" width="14.5" style="70" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="72">
+      <c r="A1" t="s" s="71">
         <v>482</v>
       </c>
-      <c r="B1" t="s" s="72">
+      <c r="B1" t="s" s="71">
         <v>33</v>
       </c>
-      <c r="C1" t="s" s="72">
+      <c r="C1" t="s" s="71">
         <v>483</v>
       </c>
-      <c r="D1" t="s" s="72">
+      <c r="D1" t="s" s="71">
         <v>484</v>
       </c>
-      <c r="E1" s="73"/>
-      <c r="F1" t="s" s="74">
+      <c r="E1" s="72"/>
+      <c r="F1" t="s" s="73">
         <v>485</v>
       </c>
-      <c r="G1" t="s" s="75">
+      <c r="G1" t="s" s="74">
         <v>486</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="76">
+      <c r="A2" t="s" s="75">
         <v>56</v>
       </c>
-      <c r="B2" t="s" s="77">
+      <c r="B2" t="s" s="76">
         <v>487</v>
       </c>
-      <c r="C2" t="s" s="78">
+      <c r="C2" t="s" s="77">
         <v>488</v>
       </c>
-      <c r="D2" t="s" s="78">
+      <c r="D2" t="s" s="77">
         <v>489</v>
       </c>
       <c r="E2" s="35"/>
@@ -23677,16 +23682,16 @@
       <c r="G2" s="24"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="76">
+      <c r="A3" t="s" s="75">
         <v>74</v>
       </c>
-      <c r="B3" t="s" s="77">
+      <c r="B3" t="s" s="76">
         <v>487</v>
       </c>
-      <c r="C3" t="s" s="78">
+      <c r="C3" t="s" s="77">
         <v>490</v>
       </c>
-      <c r="D3" t="s" s="78">
+      <c r="D3" t="s" s="77">
         <v>491</v>
       </c>
       <c r="E3" s="35"/>
@@ -23694,16 +23699,16 @@
       <c r="G3" s="8"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="76">
+      <c r="A4" t="s" s="75">
         <v>78</v>
       </c>
-      <c r="B4" t="s" s="77">
+      <c r="B4" t="s" s="76">
         <v>487</v>
       </c>
-      <c r="C4" s="79">
+      <c r="C4" s="78">
         <v>446.447</v>
       </c>
-      <c r="D4" t="s" s="80">
+      <c r="D4" t="s" s="79">
         <v>492</v>
       </c>
       <c r="E4" s="35"/>
@@ -23711,16 +23716,16 @@
       <c r="G4" s="8"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" t="s" s="76">
+      <c r="A5" t="s" s="75">
         <v>493</v>
       </c>
-      <c r="B5" t="s" s="77">
+      <c r="B5" t="s" s="76">
         <v>487</v>
       </c>
-      <c r="C5" t="s" s="78">
+      <c r="C5" t="s" s="77">
         <v>494</v>
       </c>
-      <c r="D5" t="s" s="78">
+      <c r="D5" t="s" s="77">
         <v>495</v>
       </c>
       <c r="E5" s="35"/>
@@ -23728,16 +23733,16 @@
       <c r="G5" s="8"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" t="s" s="76">
+      <c r="A6" t="s" s="75">
         <v>496</v>
       </c>
-      <c r="B6" t="s" s="77">
+      <c r="B6" t="s" s="76">
         <v>487</v>
       </c>
-      <c r="C6" t="s" s="78">
+      <c r="C6" t="s" s="77">
         <v>497</v>
       </c>
-      <c r="D6" t="s" s="80">
+      <c r="D6" t="s" s="79">
         <v>498</v>
       </c>
       <c r="E6" s="35"/>
@@ -23745,16 +23750,16 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" ht="14.5" customHeight="1">
-      <c r="A7" t="s" s="76">
+      <c r="A7" t="s" s="75">
         <v>499</v>
       </c>
-      <c r="B7" t="s" s="77">
+      <c r="B7" t="s" s="76">
         <v>487</v>
       </c>
-      <c r="C7" t="s" s="78">
+      <c r="C7" t="s" s="77">
         <v>500</v>
       </c>
-      <c r="D7" t="s" s="80">
+      <c r="D7" t="s" s="79">
         <v>501</v>
       </c>
       <c r="E7" s="35"/>
@@ -23762,16 +23767,16 @@
       <c r="G7" s="8"/>
     </row>
     <row r="8" ht="14.5" customHeight="1">
-      <c r="A8" t="s" s="76">
+      <c r="A8" t="s" s="75">
         <v>82</v>
       </c>
-      <c r="B8" t="s" s="77">
+      <c r="B8" t="s" s="76">
         <v>487</v>
       </c>
-      <c r="C8" t="s" s="78">
+      <c r="C8" t="s" s="77">
         <v>502</v>
       </c>
-      <c r="D8" t="s" s="80">
+      <c r="D8" t="s" s="79">
         <v>503</v>
       </c>
       <c r="E8" s="35"/>
@@ -23779,16 +23784,16 @@
       <c r="G8" s="8"/>
     </row>
     <row r="9" ht="14.5" customHeight="1">
-      <c r="A9" t="s" s="76">
+      <c r="A9" t="s" s="75">
         <v>504</v>
       </c>
-      <c r="B9" t="s" s="77">
+      <c r="B9" t="s" s="76">
         <v>487</v>
       </c>
-      <c r="C9" t="s" s="78">
+      <c r="C9" t="s" s="77">
         <v>505</v>
       </c>
-      <c r="D9" t="s" s="80">
+      <c r="D9" t="s" s="79">
         <v>506</v>
       </c>
       <c r="E9" s="35"/>
@@ -23796,16 +23801,16 @@
       <c r="G9" s="8"/>
     </row>
     <row r="10" ht="43.5" customHeight="1">
-      <c r="A10" t="s" s="76">
+      <c r="A10" t="s" s="75">
         <v>507</v>
       </c>
-      <c r="B10" t="s" s="77">
+      <c r="B10" t="s" s="76">
         <v>487</v>
       </c>
-      <c r="C10" t="s" s="80">
+      <c r="C10" t="s" s="79">
         <v>508</v>
       </c>
-      <c r="D10" t="s" s="78">
+      <c r="D10" t="s" s="77">
         <v>509</v>
       </c>
       <c r="E10" s="35"/>
@@ -23813,16 +23818,16 @@
       <c r="G10" s="8"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" t="s" s="76">
+      <c r="A11" t="s" s="75">
         <v>510</v>
       </c>
-      <c r="B11" t="s" s="77">
+      <c r="B11" t="s" s="76">
         <v>487</v>
       </c>
-      <c r="C11" t="s" s="78">
+      <c r="C11" t="s" s="77">
         <v>511</v>
       </c>
-      <c r="D11" t="s" s="80">
+      <c r="D11" t="s" s="79">
         <v>512</v>
       </c>
       <c r="E11" s="35"/>
@@ -23830,7 +23835,7 @@
       <c r="G11" s="8"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="81"/>
+      <c r="A12" s="80"/>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
       <c r="D12" s="44"/>
@@ -23839,7 +23844,7 @@
       <c r="G12" s="8"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="82"/>
+      <c r="A13" s="81"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -23864,48 +23869,48 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11" style="83" customWidth="1"/>
-    <col min="2" max="2" width="13.1719" style="83" customWidth="1"/>
-    <col min="3" max="5" width="8.85156" style="83" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="83" customWidth="1"/>
+    <col min="1" max="1" width="11" style="82" customWidth="1"/>
+    <col min="2" max="2" width="13.1719" style="82" customWidth="1"/>
+    <col min="3" max="5" width="8.85156" style="82" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="82" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="84">
+      <c r="A1" t="s" s="83">
         <v>51</v>
       </c>
-      <c r="B1" t="s" s="85">
+      <c r="B1" t="s" s="84">
         <v>41</v>
       </c>
-      <c r="C1" s="86"/>
+      <c r="C1" s="85"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="87">
+      <c r="A2" t="s" s="86">
         <v>64</v>
       </c>
-      <c r="B2" t="s" s="88">
-        <v>62</v>
-      </c>
-      <c r="C2" s="86"/>
+      <c r="B2" t="s" s="87">
+        <v>62</v>
+      </c>
+      <c r="C2" s="85"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="87">
+      <c r="A3" t="s" s="86">
         <v>514</v>
       </c>
-      <c r="B3" t="s" s="88">
+      <c r="B3" t="s" s="87">
         <v>63</v>
       </c>
-      <c r="C3" s="86"/>
+      <c r="C3" s="85"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="89"/>
-      <c r="B4" s="89"/>
+      <c r="A4" s="88"/>
+      <c r="B4" s="88"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>

</xml_diff>

<commit_message>
Corretti errori a seguito di mancato accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/A1111MEDUSASOFTX/Medusa_Software/Urania_FSE/v.2.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1111MEDUSASOFTX/Medusa_Software/Urania_FSE/v.2.0.0/report-checklist.xlsx
@@ -1666,13 +1666,13 @@
 </t>
   </si>
   <si>
-    <t>2025-05-13T15:55:20Z</t>
-  </si>
-  <si>
-    <t>5a2e4f06c5e4a003dd63ca3144ba541a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.97bb3fc5bee3032679f4f07419e04af6375baafa17024527a98ede920c6812ed.f198ec602c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-22T12:54:44Z</t>
+  </si>
+  <si>
+    <t>2ea742d898e5a0c507ffc40e12e6c37f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.97bb3fc5bee3032679f4f07419e04af6375baafa17024527a98ede920c6812ed.43c78e15ab^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT26_KO</t>
@@ -9079,7 +9079,7 @@
         <v>437</v>
       </c>
       <c r="F81" s="57">
-        <v>45790</v>
+        <v>45799</v>
       </c>
       <c r="G81" t="s" s="58">
         <v>438</v>

</xml_diff>